<commit_message>
add GH issues' links in field-description.html
</commit_message>
<xml_diff>
--- a/dbs/database.eamena/data/reference_data/rm/hp/mds/mds-template.xlsx
+++ b/dbs/database.eamena/data/reference_data/rm/hp/mds/mds-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rprojects\eamena-arches-dev\dbs\database.eamena\data\reference_data\mds\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rprojects\eamena-arches-dev\dbs\database.eamena\data\reference_data\rm\hp\mds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CB9B71-F404-4167-B53B-39C6BEF990F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CD1318-6A07-4BA6-AD05-5B3CC49C6893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1E0C3C69-C562-4061-B01F-1E26B463065A}"/>
   </bookViews>
@@ -156,7 +156,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="592">
   <si>
     <t>ASSESSMENT SUMMARY</t>
   </si>
@@ -1617,288 +1617,6 @@
   </si>
   <si>
     <t>7deb8fcc-c6a5-11ea-a292-02e7594ce0a0</t>
-  </si>
-  <si>
-    <t>Free text. Name and Surname of the Assessor of the heritage place</t>
-  </si>
-  <si>
-    <t>Structured data. Defines roles of the assessor within heritage management and research, including academic researchers, project staff (EAMENA, MarEA), government personnel, NGO employees, private sector workers, students/trainees, and volunteers/independent researchers.</t>
-  </si>
-  <si>
-    <t>Structured data. Delineates methods of heritage place assessment, including on-place surveys, remote image analysis, risk evaluation, emergency impact, and data processing activities.</t>
-  </si>
-  <si>
-    <t>Date. The date of the assessment</t>
-  </si>
-  <si>
-    <t>Boolean. Was the assessment based on Google Earth imagery?</t>
-  </si>
-  <si>
-    <t>Date. The date of Google Earth (GE) images used for the assessment.</t>
-  </si>
-  <si>
-    <t>Resource instance. Are Information Resources used to create and record sources (e.g., imagery, books, etc.)?</t>
-  </si>
-  <si>
-    <t>Date. The date of the acquisition of the information resource.</t>
-  </si>
-  <si>
-    <t>Free text. Name of the heritage place</t>
-  </si>
-  <si>
-    <t>Structured data. Categorises identification labels for heritage places, including alternative references, official designations, and all known toponyms across languages and periods.</t>
-  </si>
-  <si>
-    <t>Structured data. Defines categories of heritage place type, including archaeological sites, components, landscapes/seascapes, urban heritage, and structural heritage, each with specific criteria for classification.</t>
-  </si>
-  <si>
-    <t>Structured data. Outlines the types of descriptive free text for heritage places, including general place characteristics, significance summaries, architectural details, and references to previous database identifiers.</t>
-  </si>
-  <si>
-    <t>Free text. A general description of the heritage place.</t>
-  </si>
-  <si>
-    <t>Structured data. Categorises heritage places by their original or historical function, such as agricultural, defensive, domestic, leisure, funerary, hunting, water management, industrial, transport, maritime, military, public, religious, status display, and commercial activities.</t>
-  </si>
-  <si>
-    <t>Structured data. Defines the level of certainty regarding the function of heritage places, ranging from not applicable to definite, based on evidence and confirmation from various sources.</t>
-  </si>
-  <si>
-    <t>Structured list of categories indicating the status and recognition of heritage sites by various authoritative bodies and conventions.</t>
-  </si>
-  <si>
-    <t>Date. The date the heritage place was designated.</t>
-  </si>
-  <si>
-    <t>Date. The date the designation ended.</t>
-  </si>
-  <si>
-    <t>GeoJSON feature collection. The coordinates of the heritage place geometry, whether it is a point, line, or polygon.</t>
-  </si>
-  <si>
-    <t>Structured data. Describes the level of confidence in the spatial information of a heritage place, ranging from negligible to definite, based on the quality of imagery, corroborative data, and field verification.</t>
-  </si>
-  <si>
-    <t>Structured data. Defines certainty levels in identifying and delineating the boundaries of a heritage place or feature, from negligible to definite, based on imagery visibility, boundary clarity, and field corroboration.</t>
-  </si>
-  <si>
-    <t>Structured data. Describes the overall shape of heritage places, ranging from geometrically precise forms to irregular, user-defined, and unknown configurations, accommodating a variety of archaeological features.</t>
-  </si>
-  <si>
-    <t>Resource instance. EAMENA Grid ID for the location of heritage places.</t>
-  </si>
-  <si>
-    <t>Structured data. Name of the country where the heritage place is located.</t>
-  </si>
-  <si>
-    <t>Free text. Cadastral reference of the heritage place.</t>
-  </si>
-  <si>
-    <t>Structured data. Specifies the compass orientations for heritage places, including cardinal and intercardinal directions, as well as combinations for linear orientations and a category for non-applicable cases.</t>
-  </si>
-  <si>
-    <t>Free text. Address of heritage places.</t>
-  </si>
-  <si>
-    <t>Structured data. Differentiates between the main (primary) and secondary (alternative) addresses for entities in a database or record system.</t>
-  </si>
-  <si>
-    <t>Free text. Name of the administrative division of where heritage places are located.</t>
-  </si>
-  <si>
-    <t>Structured data. Categorises types of administrative divisions within a region, such as community plan areas, council districts, districts, governorates, neighborhoods, neighborhood councils, and provinces.</t>
-  </si>
-  <si>
-    <t>Structured data. Defines certainty levels in in identifying archaeological values of heritage places.</t>
-  </si>
-  <si>
-    <t>Structured data. Classifies cultural periods of cultural heritage places from Palaeolithic to Contemporary Islamic.</t>
-  </si>
-  <si>
-    <t>Structured data. Classifies the certaintiy level of chronological data associated with archaeological findings into possible, probable, definite, or not applicable, based on evidence</t>
-  </si>
-  <si>
-    <t>Structured data. Subcategories representing main cultural periods of heritage places.</t>
-  </si>
-  <si>
-    <t>Structured data. Classifies the certaintiy level of sub-periods into possible, probable, definite, or not applicable, based on evidence.</t>
-  </si>
-  <si>
-    <t>Free text. Actor involved in the process of inferring or determining dates and cultural periods and sub-periods for heritage places.</t>
-  </si>
-  <si>
-    <t>EDTF. The starting point or earliest known date of an archaeological site, a heritage place or feature, expressed in calibrated years.</t>
-  </si>
-  <si>
-    <t>EDTF. The ending point or latest known date of an archaeological site, a heritage place or feature, expressed in calibrated years.</t>
-  </si>
-  <si>
-    <t>EDTF. The starting point or earliest known date of a heritage place, expressed in years Before Present (BP).</t>
-  </si>
-  <si>
-    <t>EDTF. The ending point or latest known date of a heritage place, expressed in years Before Present (BP).</t>
-  </si>
-  <si>
-    <t>EDTF. The starting point or earliest known date of a heritage place in Anno Hijra (AH). Islamic calendar date.</t>
-  </si>
-  <si>
-    <t>EDTF. The ending point or or latest known date of a heritage place in Anno Hijra (AH). Islamic calendar date.</t>
-  </si>
-  <si>
-    <t>EDTF. The starting point or earliest known date of a heritage place in expressed in years according to the Solar Hijri (SH) calendar. The SH calendar, also known as the Persian calendar, is a solar calendar used in Iran and Afghanistan.</t>
-  </si>
-  <si>
-    <t>EDTF. The ending point or or latest known date of a heritage place in expressed in years according to the Solar Hijri (SH) calendar. The SH calendar, also known as the Persian calendar, is a solar calendar used in Iran and Afghanistan.</t>
-  </si>
-  <si>
-    <t>Structured data. Categorises physical forms and constructions of features of a heritage place, ranging from natural formations like caves to man-made structures such as walls, platforms, and mounds, based on their shape, material, and purpose.</t>
-  </si>
-  <si>
-    <t>Structured data. Measures the confidence level in feature identifications, ranging from not applicable to definite, based on evidence strength and corroboration by sources or experts.</t>
-  </si>
-  <si>
-    <t>Structured data. Describes the geometric and physical outlines of archaeological features, including shapes like circular, rectilinear, and irregular, for both enclosed and linear forms.</t>
-  </si>
-  <si>
-    <t>Structured data. Defines the spatial relationships and arrangements of archaeological features, detailing how they are positioned in relation to one another, such as isolated, linear, clustered, or concentric.</t>
-  </si>
-  <si>
-    <t>Structured data. Quantifies archaeological site complexity by the count of distinct features, ranging from singular to over five hundred, with a category for undetermined quantities.</t>
-  </si>
-  <si>
-    <t>Structured data. Defines archaeological features by their identified interpretation or type, such as structures for habitation, religious purposes, transportation, defensive mechanisms, and various processing or manufacturing activities.</t>
-  </si>
-  <si>
-    <t>Structured data. Quantifies the number of identified archaeological interpretations, from a single instance to more than five hundred, with a category for indeterminate counts.</t>
-  </si>
-  <si>
-    <t>Structured data. The level of certainty regarding the interpretation of archaeological features, ranging from negligible to definite, based on corroborative evidence and expert consensus.</t>
-  </si>
-  <si>
-    <t>Resource instance. The related Built Component resource ID pertains to heritage places and encompasses various structural and architectural elements, including walls, doors, windows, courtyards, decorative elements, etc.</t>
-  </si>
-  <si>
-    <t>Resource instance. The related Heritage Place IDs to Built Component resources (default: the one of the current Heritage Place).</t>
-  </si>
-  <si>
-    <t>Structured data. Classifies materials used in heritage places, ranging from raw materials, clay, and sediment to stone, wood, etc.</t>
-  </si>
-  <si>
-    <t>Structured data. Type of materials related to each of material classes.</t>
-  </si>
-  <si>
-    <t>Structured data. Classifies construction techniques used at heritage places, ranging from masonry, brick-laid laying, and beam-supported to wood construction, roofing, etc.</t>
-  </si>
-  <si>
-    <t>Free text. Measurement numeric value of heritage places.</t>
-  </si>
-  <si>
-    <t>Structured data. Describes types of spatial measurements for sites or features, including area, breadth/width, depth, diameter, height, length, and an 'unknown' category for unspecified dimensions.</t>
-  </si>
-  <si>
-    <t>Structured data. Identifies the methods used to obtain measurements of sites or features, such as imagery analysis, various forms of aerial photography, satellite imagery, field surveys, GPS technologies, pacing estimations, laser rangefinders, tape measures, total stations, theodolites, or unspecified sources.</t>
-  </si>
-  <si>
-    <t>Resource instance. The related Geoarchaeology resource ID related to heritage places.</t>
-  </si>
-  <si>
-    <t>Structured data. Evaluates the preservation state of heritage places, from 'good' indicating minimal damage, to 'destroyed' where integrity is lost and data is no longer retrievable.</t>
-  </si>
-  <si>
-    <t>Structured data. Describes the scope of damage or disturbance at heritage places, with categories ranging from no visible damage to near-total visible damage.</t>
-  </si>
-  <si>
-    <t>Structured data: Describes categories of disturbance caused at heritage places, ranging from Agricultural/Pastoral, Building/Development, Natural, and Domestic Use to Infrastructure/Transport, Looting/Illegal activities, Military/Armed Conflict, etc.</t>
-  </si>
-  <si>
-    <t>Structured data. Determines the type of disturbance causes related to each of the cause categories, ranging from animal/pest infestation to wind and water action.</t>
-  </si>
-  <si>
-    <t>Structured data. Determines the confidence level in identifying the cause of disturbance to heritage places, from 'not applicable' to 'definite', based on the evidence and expert agreement.</t>
-  </si>
-  <si>
-    <t>Date. Event occurred at some point between two dates - enter the date span</t>
-  </si>
-  <si>
-    <t>Date. Event occurred before a specific date. The 'from' field does not apply.</t>
-  </si>
-  <si>
-    <t>Date. Event occurred on a specific date.</t>
-  </si>
-  <si>
-    <t>Free text. the name of the assessor or actor who identified and recorded the disturbance cause.</t>
-  </si>
-  <si>
-    <t>Structured data. Outlines various impacts on heritage places, ranging from access restriction to water damage, including physical alterations, chemical effects, and loss of heritage materials or value.</t>
-  </si>
-  <si>
-    <t>Structured data. Assesses the confidence in determining the effects of disturbance on heritage placess, ranging from 'not applicable' when uncertain, to 'definite' when confirmed by evidence and experts.</t>
-  </si>
-  <si>
-    <t>Structured data. Classifies potential future risks to heritage places, from agricultural impact to military conflict, including environmental and illicit threats, as well as societal and infrastructural pressures.</t>
-  </si>
-  <si>
-    <t>Structured data. Details the array of potential threats (future disturbances) to heritage sites, encompassing natural processes, human activities, and environmental changes that can cause damage or alteration.</t>
-  </si>
-  <si>
-    <t>Structured data. Assesses the likelihood of future threats to heritage places, with categories ranging from 'not applicable' to 'planned', considering factors like proximity and the nature of the threat.</t>
-  </si>
-  <si>
-    <t>Free text. The name of the assessor or actor who identified and recorded the threats.</t>
-  </si>
-  <si>
-    <t>Structured data. Classifies types of activities for heritage place protection, including emergency interventions, conservation and restoration efforts, and preventative measures.</t>
-  </si>
-  <si>
-    <t>Structured data. Defines detailed activities related to identified intervention types for managing and preserving heritage places, ranging from surveys and excavations to conservation and maintenance practices, as well as management and preventive strategies.</t>
-  </si>
-  <si>
-    <t>Structured data. Categorises urgency levels for action at heritage places, from 'emergency' requiring immediate attention to 'low' priority where long-term planning is possible.</t>
-  </si>
-  <si>
-    <t>Resource instance. Detailed Condition Resource ID related to heritage places</t>
-  </si>
-  <si>
-    <t>Structured data. Details various landforms and water-related features in relation to heritage sites, including alluvial fans, lake beds, shores, sea beds, bays, beaches, cliffs, deltas, estuaries, intertidal flats, islands, reefs, plains, plateaus, precipices, slopes, summits, valleys, terraces, and watercourse edges and beds.</t>
-  </si>
-  <si>
-    <t>Structured data. Categorises the predominant type of surface cover at heritage sites, ranging from various vegetation types and water bodies to barren lands and built-up areas.</t>
-  </si>
-  <si>
-    <t>Date. The date of the land cover assessment.</t>
-  </si>
-  <si>
-    <t>Structured data. Describes surface geological materials, from coarse sediments and mixed deposits to mud, organic materials, paleontological remains, rocks, boulders, sand, and archaeological layers, highlighting composition and grain size.</t>
-  </si>
-  <si>
-    <t>Structured data. Outlines types of sediment deposition processes, from aeolian (wind) and biogenic (organism-produced) to chemical, fluvial, glacial, and marine, including volcanic and anthropogenic influences on sedimentation.</t>
-  </si>
-  <si>
-    <t>Structured data. Classifies types of bedrock geology, detailing igneous, sedimentary, and metamorphic rocks, with specific examples like basalt, granite, limestone, marble, and others, including undefined categories for unspecified types.</t>
-  </si>
-  <si>
-    <t>Structured data. Defines coastal exposure levels based on fetch, the straight-line distance over water from a coast to the nearest landmass, with categories for exposed, moderately exposed, and protected environments.</t>
-  </si>
-  <si>
-    <t>Structured data. Dominant wave patterns and influences by monsoons, protection, storms, swells, tides, or cyclones.</t>
-  </si>
-  <si>
-    <t>Structured data. Vertical height difference between high and low tide.</t>
-  </si>
-  <si>
-    <t>Free text. The minimum depth (i.e., maximum elevation) numeric value (in meter)</t>
-  </si>
-  <si>
-    <t>Free text. The maximum depth (i.e., minimum elevation) numeric value (in meter)</t>
-  </si>
-  <si>
-    <t>Structured data. The datum of the Depth/Elevation (Biological Mean Sea Level, Mean High Water, etc.).</t>
-  </si>
-  <si>
-    <t>Free text. The EPSG code of the coordinates.</t>
-  </si>
-  <si>
-    <t>Depreciated</t>
   </si>
   <si>
     <t>num</t>
@@ -1919,18 +1637,9 @@
     </r>
   </si>
   <si>
-    <t>Structured data. The type of geometry qualifier, whether it is Centre Point, Access Point, Buffer Polygon, Center Line, Facade Point, Perimeter Polygon, Property Boundary, Site Datum Point, Simplified Polygon, or Vicinity Point.</t>
-  </si>
-  <si>
-    <t>Structured data. Identifies types of heritage places based on their morphology - whether they are negative/cut/dug features, constructed above ground, surface marks, or undetermined.</t>
-  </si>
-  <si>
     <t>Yes (Including 'Unknown')</t>
   </si>
   <si>
-    <t>Structured data. Categorises units of measurement of heritage places by system: Metric (mm, cm, m, km, ha, m2, km2), Imperial (in, ft, yd, mi, ac, ft2, mi2), and Other (dunam).</t>
-  </si>
-  <si>
     <t>Yes (including 'Unknown')</t>
   </si>
   <si>
@@ -1941,13 +1650,307 @@
   </si>
   <si>
     <t>e3cc8c5b-c772-11ea-a292-02e7594ce0a0</t>
+  </si>
+  <si>
+    <t>Structured data. Defines roles of the assessor within heritage management and research, including academic researchers, project staff (EAMENA, MarEA), government personnel, NGO employees, private sector workers, students/trainees, and volunteers/independent researchers. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/60'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Delineates methods of heritage place assessment, including on-place surveys, remote image analysis, risk evaluation, emergency impact, and data processing activities. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/61'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Boolean. Was the assessment based on Google Earth imagery? &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/63'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Date. The date of Google Earth (GE) images used for the assessment. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/64'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Resource instance. Are Information Resources used to create and record sources (e.g., imagery, books, etc.)? &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/65'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Date. The date of the acquisition of the information resource. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/66'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Categorises identification labels for heritage places, including alternative references, official designations, and all known toponyms across languages and periods. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/68'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Defines categories of heritage place type, including archaeological sites, components, landscapes/seascapes, urban heritage, and structural heritage, each with specific criteria for classification. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/69'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Outlines the types of descriptive free text for heritage places, including general place characteristics, significance summaries, architectural details, and references to previous database identifiers. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/70'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Free text. A general description of the heritage place. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/71'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Categorises heritage places by their original or historical function, such as agricultural, defensive, domestic, leisure, funerary, hunting, water management, industrial, transport, maritime, military, public, religious, status display, and commercial activities. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/72'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Defines the level of certainty regarding the function of heritage places, ranging from not applicable to definite, based on evidence and confirmation from various sources. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/73'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured list of categories indicating the status and recognition of heritage sites by various authoritative bodies and conventions. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/74'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Date. The date the heritage place was designated. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/75'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Date. The date the designation ended. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/76'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>GeoJSON feature collection. The coordinates of the heritage place geometry, whether it is a point, line, or polygon. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/77'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. The type of geometry qualifier, whether it is Centre Point, Access Point, Buffer Polygon, Center Line, Facade Point, Perimeter Polygon, Property Boundary, Site Datum Point, Simplified Polygon, or Vicinity Point. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/78'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Describes the level of confidence in the spatial information of a heritage place, ranging from negligible to definite, based on the quality of imagery, corroborative data, and field verification. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/79'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Defines certainty levels in identifying and delineating the boundaries of a heritage place or feature, from negligible to definite, based on imagery visibility, boundary clarity, and field corroboration. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/80'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Describes the overall shape of heritage places, ranging from geometrically precise forms to irregular, user-defined, and unknown configurations, accommodating a variety of archaeological features. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/81'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Resource instance. EAMENA Grid ID for the location of heritage places. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/82'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Name of the country where the heritage place is located. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/83'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Free text. Cadastral reference of the heritage place. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/84'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Specifies the compass orientations for heritage places, including cardinal and intercardinal directions, as well as combinations for linear orientations and a category for non-applicable cases. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/85'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Free text. Address of heritage places. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/86'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Differentiates between the main (primary) and secondary (alternative) addresses for entities in a database or record system. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/87'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Free text. Name of the administrative division of where heritage places are located. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/88'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Categorises types of administrative divisions within a region, such as community plan areas, council districts, districts, governorates, neighborhoods, neighborhood councils, and provinces. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/89'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Defines certainty levels in in identifying archaeological values of heritage places. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/90'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Identifies types of heritage places based on their morphology - whether they are negative/cut/dug features, constructed above ground, surface marks, or undetermined. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/91'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Classifies cultural periods of cultural heritage places from Palaeolithic to Contemporary Islamic. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/92'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Classifies the certaintiy level of chronological data associated with archaeological findings into possible, probable, definite, or not applicable, based on evidence &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/93'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Subcategories representing main cultural periods of heritage places. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/94'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Classifies the certaintiy level of sub-periods into possible, probable, definite, or not applicable, based on evidence. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/95'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Free text. Actor involved in the process of inferring or determining dates and cultural periods and sub-periods for heritage places. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/96'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>EDTF. The starting point or earliest known date of an archaeological site, a heritage place or feature, expressed in calibrated years. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/97'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>EDTF. The ending point or latest known date of an archaeological site, a heritage place or feature, expressed in calibrated years. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/98'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>EDTF. The starting point or earliest known date of a heritage place, expressed in years Before Present (BP). &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/99'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>EDTF. The ending point or latest known date of a heritage place, expressed in years Before Present (BP). &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/100'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>EDTF. The starting point or earliest known date of a heritage place in Anno Hijra (AH). Islamic calendar date. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/101'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>EDTF. The ending point or or latest known date of a heritage place in Anno Hijra (AH). Islamic calendar date. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/102'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>EDTF. The starting point or earliest known date of a heritage place in expressed in years according to the Solar Hijri (SH) calendar. The SH calendar, also known as the Persian calendar, is a solar calendar used in Iran and Afghanistan. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/103'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>EDTF. The ending point or or latest known date of a heritage place in expressed in years according to the Solar Hijri (SH) calendar. The SH calendar, also known as the Persian calendar, is a solar calendar used in Iran and Afghanistan. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/104'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Categorises physical forms and constructions of features of a heritage place, ranging from natural formations like caves to man-made structures such as walls, platforms, and mounds, based on their shape, material, and purpose. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/105'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Measures the confidence level in feature identifications, ranging from not applicable to definite, based on evidence strength and corroboration by sources or experts. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/106'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Describes the geometric and physical outlines of archaeological features, including shapes like circular, rectilinear, and irregular, for both enclosed and linear forms. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/107'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Defines the spatial relationships and arrangements of archaeological features, detailing how they are positioned in relation to one another, such as isolated, linear, clustered, or concentric. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/108'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Quantifies archaeological site complexity by the count of distinct features, ranging from singular to over five hundred, with a category for undetermined quantities. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/109'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Defines archaeological features by their identified interpretation or type, such as structures for habitation, religious purposes, transportation, defensive mechanisms, and various processing or manufacturing activities. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/110'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Quantifies the number of identified archaeological interpretations, from a single instance to more than five hundred, with a category for indeterminate counts. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/111'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. The level of certainty regarding the interpretation of archaeological features, ranging from negligible to definite, based on corroborative evidence and expert consensus. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/112'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Resource instance. The related Built Component resource ID pertains to heritage places and encompasses various structural and architectural elements, including walls, doors, windows, courtyards, decorative elements, etc. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/113'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Resource instance. The related Heritage Place IDs to Built Component resources (default: the one of the current Heritage Place). &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/114'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Classifies materials used in heritage places, ranging from raw materials, clay, and sediment to stone, wood, etc. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/115'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Type of materials related to each of material classes. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/116'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Classifies construction techniques used at heritage places, ranging from masonry, brick-laid laying, and beam-supported to wood construction, roofing, etc. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/117'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Free text. Measurement numeric value of heritage places. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/118'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Categorises units of measurement of heritage places by system: Metric (mm, cm, m, km, ha, m2, km2), Imperial (in, ft, yd, mi, ac, ft2, mi2), and Other (dunam). &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/119'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Describes types of spatial measurements for sites or features, including area, breadth/width, depth, diameter, height, length, and an 'unknown' category for unspecified dimensions. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/120'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Identifies the methods used to obtain measurements of sites or features, such as imagery analysis, various forms of aerial photography, satellite imagery, field surveys, GPS technologies, pacing estimations, laser rangefinders, tape measures, total stations, theodolites, or unspecified sources. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/121'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Resource instance. The related Geoarchaeology resource ID related to heritage places. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/122'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Evaluates the preservation state of heritage places, from 'good' indicating minimal damage, to 'destroyed' where integrity is lost and data is no longer retrievable. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/123'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Describes the scope of damage or disturbance at heritage places, with categories ranging from no visible damage to near-total visible damage. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/124'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data: Describes categories of disturbance caused at heritage places, ranging from Agricultural/Pastoral, Building/Development, Natural, and Domestic Use to Infrastructure/Transport, Looting/Illegal activities, Military/Armed Conflict, etc. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/125'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Determines the type of disturbance causes related to each of the cause categories, ranging from animal/pest infestation to wind and water action. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/126'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Determines the confidence level in identifying the cause of disturbance to heritage places, from 'not applicable' to 'definite', based on the evidence and expert agreement. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/127'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Date. Event occurred before a specific date. The 'from' field does not apply. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/130'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Date. Event occurred on a specific date. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/131'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Free text. the name of the assessor or actor who identified and recorded the disturbance cause. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/132'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Outlines various impacts on heritage places, ranging from access restriction to water damage, including physical alterations, chemical effects, and loss of heritage materials or value. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/133'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Assesses the confidence in determining the effects of disturbance on heritage placess, ranging from 'not applicable' when uncertain, to 'definite' when confirmed by evidence and experts. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/134'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Classifies potential future risks to heritage places, from agricultural impact to military conflict, including environmental and illicit threats, as well as societal and infrastructural pressures. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/135'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Details the array of potential threats (future disturbances) to heritage sites, encompassing natural processes, human activities, and environmental changes that can cause damage or alteration. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/136'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Assesses the likelihood of future threats to heritage places, with categories ranging from 'not applicable' to 'planned', considering factors like proximity and the nature of the threat. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/137'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Free text. The name of the assessor or actor who identified and recorded the threats. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/138'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Classifies types of activities for heritage place protection, including emergency interventions, conservation and restoration efforts, and preventative measures. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/139'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Defines detailed activities related to identified intervention types for managing and preserving heritage places, ranging from surveys and excavations to conservation and maintenance practices, as well as management and preventive strategies. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/140'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Categorises urgency levels for action at heritage places, from 'emergency' requiring immediate attention to 'low' priority where long-term planning is possible. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/141'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Details various landforms and water-related features in relation to heritage sites, including alluvial fans, lake beds, shores, sea beds, bays, beaches, cliffs, deltas, estuaries, intertidal flats, islands, reefs, plains, plateaus, precipices, slopes, summits, valleys, terraces, and watercourse edges and beds. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/143'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Categorises the predominant type of surface cover at heritage sites, ranging from various vegetation types and water bodies to barren lands and built-up areas. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/144'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Date. The date of the land cover assessment. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/145'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Describes surface geological materials, from coarse sediments and mixed deposits to mud, organic materials, paleontological remains, rocks, boulders, sand, and archaeological layers, highlighting composition and grain size. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/146'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Outlines types of sediment deposition processes, from aeolian (wind) and biogenic (organism-produced) to chemical, fluvial, glacial, and marine, including volcanic and anthropogenic influences on sedimentation. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/147'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Classifies types of bedrock geology, detailing igneous, sedimentary, and metamorphic rocks, with specific examples like basalt, granite, limestone, marble, and others, including undefined categories for unspecified types. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/148'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Defines coastal exposure levels based on fetch, the straight-line distance over water from a coast to the nearest landmass, with categories for exposed, moderately exposed, and protected environments. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/149'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Dominant wave patterns and influences by monsoons, protection, storms, swells, tides, or cyclones. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/150'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Vertical height difference between high and low tide. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/151'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. The datum of the Depth/Elevation (Biological Mean Sea Level, Mean High Water, etc.). &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/154'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Free text. The EPSG code of the coordinates. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/155'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Free text. Name and Surname of the Assessor of the heritage place. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/59'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Date. The date of the assessment. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/62'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Free text. Name of the heritage place. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/67'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Date. Event occurred at some point between two dates - enter the date span. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/128'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Date. Event occurred at some point between two dates - enter the date span. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/129'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Resource instance. Detailed Condition Resource ID related to heritage places. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/142'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Depreciated. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/156'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Free text. The maximum depth (i.e., minimum elevation) numeric value (in meter). &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/153'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Free text. The minimum depth (i.e., maximum elevation) numeric value (in meter). &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/152'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2015,24 +2018,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF374151"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -2232,7 +2217,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2358,12 +2343,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="20% - Accent2 2" xfId="5" xr:uid="{1DC40975-83D9-45B2-A3A5-0EB98FC5D267}"/>
@@ -2416,9 +2395,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2456,7 +2435,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2562,7 +2541,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2704,7 +2683,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2755,11 +2734,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42076D7F-BEF1-41ED-B129-2E241988AEAC}">
   <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E70" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="H73" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E73" sqref="E73"/>
+      <selection pane="bottomRight" activeCell="H96" sqref="H96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2767,7 +2746,7 @@
     <col min="1" max="1" width="4.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.77734375" style="38" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.109375" style="38" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.109375" style="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.44140625" style="38" customWidth="1"/>
     <col min="5" max="5" width="36" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="67.109375" customWidth="1"/>
     <col min="7" max="7" width="27.33203125" customWidth="1"/>
@@ -2777,7 +2756,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>581</v>
+        <v>487</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>91</v>
@@ -2804,7 +2783,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2823,14 +2802,14 @@
       <c r="F2" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="H2" s="45" t="s">
-        <v>487</v>
+      <c r="H2" t="s">
+        <v>583</v>
       </c>
       <c r="I2" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2849,14 +2828,14 @@
       <c r="F3" t="s">
         <v>106</v>
       </c>
-      <c r="H3" s="46" t="s">
-        <v>488</v>
+      <c r="H3" t="s">
+        <v>494</v>
       </c>
       <c r="I3" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2875,14 +2854,14 @@
       <c r="F4" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="H4" s="45" t="s">
-        <v>489</v>
+      <c r="H4" t="s">
+        <v>495</v>
       </c>
       <c r="I4" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2901,14 +2880,14 @@
       <c r="F5" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="H5" s="45" t="s">
-        <v>490</v>
+      <c r="H5" t="s">
+        <v>584</v>
       </c>
       <c r="I5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2927,14 +2906,14 @@
       <c r="F6" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="H6" s="45" t="s">
-        <v>491</v>
+      <c r="H6" t="s">
+        <v>496</v>
       </c>
       <c r="I6" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2953,14 +2932,14 @@
       <c r="F7" t="s">
         <v>107</v>
       </c>
-      <c r="H7" s="45" t="s">
-        <v>492</v>
+      <c r="H7" t="s">
+        <v>497</v>
       </c>
       <c r="I7" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2976,14 +2955,14 @@
       <c r="E8" t="s">
         <v>176</v>
       </c>
-      <c r="H8" s="45" t="s">
-        <v>493</v>
+      <c r="H8" t="s">
+        <v>498</v>
       </c>
       <c r="I8" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2999,14 +2978,14 @@
       <c r="E9" t="s">
         <v>101</v>
       </c>
-      <c r="H9" s="45" t="s">
-        <v>494</v>
+      <c r="H9" t="s">
+        <v>499</v>
       </c>
       <c r="I9" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3025,14 +3004,14 @@
       <c r="F10" t="s">
         <v>108</v>
       </c>
-      <c r="H10" s="45" t="s">
-        <v>495</v>
+      <c r="H10" t="s">
+        <v>585</v>
       </c>
       <c r="I10" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3051,14 +3030,14 @@
       <c r="F11" t="s">
         <v>109</v>
       </c>
-      <c r="H11" s="45" t="s">
-        <v>496</v>
+      <c r="H11" t="s">
+        <v>500</v>
       </c>
       <c r="I11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3077,14 +3056,14 @@
       <c r="F12" t="s">
         <v>110</v>
       </c>
-      <c r="H12" s="45" t="s">
-        <v>497</v>
+      <c r="H12" t="s">
+        <v>501</v>
       </c>
       <c r="I12" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3103,14 +3082,14 @@
       <c r="F13" t="s">
         <v>110</v>
       </c>
-      <c r="H13" s="45" t="s">
-        <v>498</v>
+      <c r="H13" t="s">
+        <v>502</v>
       </c>
       <c r="I13" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3129,14 +3108,14 @@
       <c r="F14" t="s">
         <v>110</v>
       </c>
-      <c r="H14" s="45" t="s">
-        <v>499</v>
+      <c r="H14" t="s">
+        <v>503</v>
       </c>
       <c r="I14" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3153,16 +3132,16 @@
         <v>117</v>
       </c>
       <c r="F15" t="s">
-        <v>582</v>
-      </c>
-      <c r="H15" s="45" t="s">
-        <v>500</v>
+        <v>488</v>
+      </c>
+      <c r="H15" t="s">
+        <v>504</v>
       </c>
       <c r="I15" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3181,14 +3160,14 @@
       <c r="F16" t="s">
         <v>111</v>
       </c>
-      <c r="H16" s="45" t="s">
-        <v>501</v>
+      <c r="H16" t="s">
+        <v>505</v>
       </c>
       <c r="I16" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3207,14 +3186,14 @@
       <c r="F17" t="s">
         <v>110</v>
       </c>
-      <c r="H17" s="45" t="s">
-        <v>502</v>
+      <c r="H17" t="s">
+        <v>506</v>
       </c>
       <c r="I17" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3233,14 +3212,14 @@
       <c r="F18" t="s">
         <v>110</v>
       </c>
-      <c r="H18" s="45" t="s">
-        <v>503</v>
+      <c r="H18" t="s">
+        <v>507</v>
       </c>
       <c r="I18" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3259,14 +3238,14 @@
       <c r="F19" t="s">
         <v>110</v>
       </c>
-      <c r="H19" s="45" t="s">
-        <v>504</v>
+      <c r="H19" t="s">
+        <v>508</v>
       </c>
       <c r="I19" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3285,14 +3264,14 @@
       <c r="F20" t="s">
         <v>106</v>
       </c>
-      <c r="H20" s="45" t="s">
-        <v>505</v>
+      <c r="H20" t="s">
+        <v>509</v>
       </c>
       <c r="I20" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3308,14 +3287,14 @@
       <c r="E21" t="s">
         <v>121</v>
       </c>
-      <c r="H21" s="45" t="s">
-        <v>583</v>
+      <c r="H21" t="s">
+        <v>510</v>
       </c>
       <c r="I21" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3334,14 +3313,14 @@
       <c r="F22" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="H22" s="45" t="s">
-        <v>506</v>
+      <c r="H22" t="s">
+        <v>511</v>
       </c>
       <c r="I22" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3360,14 +3339,14 @@
       <c r="F23" t="s">
         <v>110</v>
       </c>
-      <c r="H23" s="45" t="s">
-        <v>507</v>
+      <c r="H23" t="s">
+        <v>512</v>
       </c>
       <c r="I23" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3386,14 +3365,14 @@
       <c r="F24" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="H24" s="45" t="s">
-        <v>508</v>
+      <c r="H24" t="s">
+        <v>513</v>
       </c>
       <c r="I24" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3412,14 +3391,14 @@
       <c r="F25" t="s">
         <v>106</v>
       </c>
-      <c r="H25" s="45" t="s">
-        <v>509</v>
+      <c r="H25" t="s">
+        <v>514</v>
       </c>
       <c r="I25" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3438,14 +3417,14 @@
       <c r="F26" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="H26" s="45" t="s">
-        <v>510</v>
+      <c r="H26" t="s">
+        <v>515</v>
       </c>
       <c r="I26" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3464,14 +3443,14 @@
       <c r="F27" t="s">
         <v>110</v>
       </c>
-      <c r="H27" s="45" t="s">
-        <v>511</v>
+      <c r="H27" t="s">
+        <v>516</v>
       </c>
       <c r="I27" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3490,14 +3469,14 @@
       <c r="F28" t="s">
         <v>110</v>
       </c>
-      <c r="H28" s="45" t="s">
-        <v>512</v>
+      <c r="H28" t="s">
+        <v>517</v>
       </c>
       <c r="I28" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3513,14 +3492,14 @@
       <c r="E29" t="s">
         <v>127</v>
       </c>
-      <c r="H29" s="45" t="s">
-        <v>513</v>
+      <c r="H29" t="s">
+        <v>518</v>
       </c>
       <c r="I29" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3536,14 +3515,14 @@
       <c r="E30" t="s">
         <v>128</v>
       </c>
-      <c r="H30" s="45" t="s">
-        <v>514</v>
+      <c r="H30" t="s">
+        <v>519</v>
       </c>
       <c r="I30" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3559,14 +3538,14 @@
       <c r="E31" t="s">
         <v>182</v>
       </c>
-      <c r="H31" s="45" t="s">
-        <v>515</v>
+      <c r="H31" t="s">
+        <v>520</v>
       </c>
       <c r="I31" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3582,14 +3561,14 @@
       <c r="E32" t="s">
         <v>183</v>
       </c>
-      <c r="H32" s="45" t="s">
-        <v>516</v>
+      <c r="H32" t="s">
+        <v>521</v>
       </c>
       <c r="I32" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3608,14 +3587,14 @@
       <c r="F33" t="s">
         <v>106</v>
       </c>
-      <c r="H33" s="45" t="s">
-        <v>517</v>
+      <c r="H33" t="s">
+        <v>522</v>
       </c>
       <c r="I33" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3634,14 +3613,14 @@
       <c r="F34" t="s">
         <v>106</v>
       </c>
-      <c r="H34" s="45" t="s">
-        <v>584</v>
+      <c r="H34" t="s">
+        <v>523</v>
       </c>
       <c r="I34" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3658,16 +3637,16 @@
         <v>130</v>
       </c>
       <c r="F35" s="39" t="s">
-        <v>585</v>
-      </c>
-      <c r="H35" s="45" t="s">
-        <v>518</v>
+        <v>489</v>
+      </c>
+      <c r="H35" t="s">
+        <v>524</v>
       </c>
       <c r="I35" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3686,14 +3665,14 @@
       <c r="F36" t="s">
         <v>106</v>
       </c>
-      <c r="H36" s="45" t="s">
-        <v>519</v>
+      <c r="H36" t="s">
+        <v>525</v>
       </c>
       <c r="I36" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3712,14 +3691,14 @@
       <c r="F37" t="s">
         <v>110</v>
       </c>
-      <c r="H37" s="45" t="s">
-        <v>520</v>
+      <c r="H37" t="s">
+        <v>526</v>
       </c>
       <c r="I37" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3738,14 +3717,14 @@
       <c r="F38" t="s">
         <v>110</v>
       </c>
-      <c r="H38" s="45" t="s">
-        <v>521</v>
+      <c r="H38" t="s">
+        <v>527</v>
       </c>
       <c r="I38" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3761,14 +3740,14 @@
       <c r="E39" t="s">
         <v>132</v>
       </c>
-      <c r="H39" s="45" t="s">
-        <v>522</v>
+      <c r="H39" t="s">
+        <v>528</v>
       </c>
       <c r="I39" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3784,14 +3763,14 @@
       <c r="E40" t="s">
         <v>193</v>
       </c>
-      <c r="H40" s="45" t="s">
-        <v>523</v>
+      <c r="H40" t="s">
+        <v>529</v>
       </c>
       <c r="I40" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3807,14 +3786,14 @@
       <c r="E41" t="s">
         <v>194</v>
       </c>
-      <c r="H41" s="45" t="s">
-        <v>524</v>
+      <c r="H41" t="s">
+        <v>530</v>
       </c>
       <c r="I41" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3830,14 +3809,14 @@
       <c r="E42" t="s">
         <v>133</v>
       </c>
-      <c r="H42" s="45" t="s">
-        <v>525</v>
+      <c r="H42" t="s">
+        <v>531</v>
       </c>
       <c r="I42" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3853,14 +3832,14 @@
       <c r="E43" t="s">
         <v>134</v>
       </c>
-      <c r="H43" s="45" t="s">
-        <v>526</v>
+      <c r="H43" t="s">
+        <v>532</v>
       </c>
       <c r="I43" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3876,14 +3855,14 @@
       <c r="E44" t="s">
         <v>135</v>
       </c>
-      <c r="H44" s="45" t="s">
-        <v>527</v>
+      <c r="H44" t="s">
+        <v>533</v>
       </c>
       <c r="I44" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3899,14 +3878,14 @@
       <c r="E45" t="s">
         <v>136</v>
       </c>
-      <c r="H45" s="45" t="s">
-        <v>528</v>
+      <c r="H45" t="s">
+        <v>534</v>
       </c>
       <c r="I45" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3922,14 +3901,14 @@
       <c r="E46" t="s">
         <v>137</v>
       </c>
-      <c r="H46" s="45" t="s">
-        <v>529</v>
+      <c r="H46" t="s">
+        <v>535</v>
       </c>
       <c r="I46" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3945,14 +3924,14 @@
       <c r="E47" t="s">
         <v>197</v>
       </c>
-      <c r="H47" s="45" t="s">
-        <v>530</v>
+      <c r="H47" t="s">
+        <v>536</v>
       </c>
       <c r="I47" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3971,14 +3950,14 @@
       <c r="F48" t="s">
         <v>112</v>
       </c>
-      <c r="H48" s="45" t="s">
-        <v>531</v>
+      <c r="H48" t="s">
+        <v>537</v>
       </c>
       <c r="I48" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3997,14 +3976,14 @@
       <c r="F49" t="s">
         <v>109</v>
       </c>
-      <c r="H49" s="45" t="s">
-        <v>532</v>
+      <c r="H49" t="s">
+        <v>538</v>
       </c>
       <c r="I49" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4023,14 +4002,14 @@
       <c r="F50" t="s">
         <v>110</v>
       </c>
-      <c r="H50" s="45" t="s">
-        <v>533</v>
+      <c r="H50" t="s">
+        <v>539</v>
       </c>
       <c r="I50" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4049,14 +4028,14 @@
       <c r="F51" t="s">
         <v>110</v>
       </c>
-      <c r="H51" s="45" t="s">
-        <v>534</v>
+      <c r="H51" t="s">
+        <v>540</v>
       </c>
       <c r="I51" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4075,14 +4054,14 @@
       <c r="F52" t="s">
         <v>110</v>
       </c>
-      <c r="H52" s="45" t="s">
-        <v>535</v>
+      <c r="H52" t="s">
+        <v>541</v>
       </c>
       <c r="I52" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4099,16 +4078,16 @@
         <v>198</v>
       </c>
       <c r="F53" s="42" t="s">
-        <v>587</v>
-      </c>
-      <c r="H53" s="45" t="s">
-        <v>536</v>
+        <v>490</v>
+      </c>
+      <c r="H53" t="s">
+        <v>542</v>
       </c>
       <c r="I53" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4127,14 +4106,14 @@
       <c r="F54" t="s">
         <v>106</v>
       </c>
-      <c r="H54" s="45" t="s">
-        <v>537</v>
+      <c r="H54" t="s">
+        <v>543</v>
       </c>
       <c r="I54" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4153,14 +4132,14 @@
       <c r="F55" t="s">
         <v>106</v>
       </c>
-      <c r="H55" s="45" t="s">
-        <v>538</v>
+      <c r="H55" t="s">
+        <v>544</v>
       </c>
       <c r="I55" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4179,14 +4158,14 @@
       <c r="G56" t="s">
         <v>205</v>
       </c>
-      <c r="H56" s="45" t="s">
-        <v>539</v>
+      <c r="H56" t="s">
+        <v>545</v>
       </c>
       <c r="I56" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4205,14 +4184,14 @@
       <c r="G57" t="s">
         <v>205</v>
       </c>
-      <c r="H57" s="45" t="s">
-        <v>540</v>
+      <c r="H57" t="s">
+        <v>546</v>
       </c>
       <c r="I57" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4228,14 +4207,14 @@
       <c r="E58" t="s">
         <v>144</v>
       </c>
-      <c r="H58" s="45" t="s">
-        <v>541</v>
+      <c r="H58" t="s">
+        <v>547</v>
       </c>
       <c r="I58" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4251,14 +4230,14 @@
       <c r="E59" t="s">
         <v>145</v>
       </c>
-      <c r="H59" s="45" t="s">
-        <v>542</v>
+      <c r="H59" t="s">
+        <v>548</v>
       </c>
       <c r="I59" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4274,14 +4253,14 @@
       <c r="E60" t="s">
         <v>146</v>
       </c>
-      <c r="H60" s="47" t="s">
-        <v>543</v>
+      <c r="H60" t="s">
+        <v>549</v>
       </c>
       <c r="I60" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4297,14 +4276,14 @@
       <c r="E61" t="s">
         <v>147</v>
       </c>
-      <c r="H61" s="45" t="s">
-        <v>544</v>
+      <c r="H61" t="s">
+        <v>550</v>
       </c>
       <c r="I61" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4320,14 +4299,14 @@
       <c r="E62" t="s">
         <v>148</v>
       </c>
-      <c r="H62" s="45" t="s">
-        <v>586</v>
+      <c r="H62" t="s">
+        <v>551</v>
       </c>
       <c r="I62" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4343,14 +4322,14 @@
       <c r="E63" t="s">
         <v>149</v>
       </c>
-      <c r="H63" s="45" t="s">
-        <v>545</v>
+      <c r="H63" t="s">
+        <v>552</v>
       </c>
       <c r="I63" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4366,14 +4345,14 @@
       <c r="E64" t="s">
         <v>206</v>
       </c>
-      <c r="H64" s="45" t="s">
-        <v>546</v>
+      <c r="H64" t="s">
+        <v>553</v>
       </c>
       <c r="I64" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4392,14 +4371,14 @@
       <c r="F65" t="s">
         <v>110</v>
       </c>
-      <c r="H65" s="45" t="s">
-        <v>547</v>
+      <c r="H65" t="s">
+        <v>554</v>
       </c>
       <c r="I65" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4418,14 +4397,14 @@
       <c r="F66" t="s">
         <v>113</v>
       </c>
-      <c r="H66" s="45" t="s">
-        <v>548</v>
+      <c r="H66" t="s">
+        <v>555</v>
       </c>
       <c r="I66" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4444,14 +4423,14 @@
       <c r="F67" t="s">
         <v>110</v>
       </c>
-      <c r="H67" s="45" t="s">
-        <v>549</v>
+      <c r="H67" t="s">
+        <v>556</v>
       </c>
       <c r="I67" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4470,14 +4449,14 @@
       <c r="F68" t="s">
         <v>113</v>
       </c>
-      <c r="H68" s="45" t="s">
-        <v>550</v>
+      <c r="H68" t="s">
+        <v>557</v>
       </c>
       <c r="I68" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4496,14 +4475,14 @@
       <c r="F69" t="s">
         <v>113</v>
       </c>
-      <c r="H69" s="47" t="s">
-        <v>551</v>
+      <c r="H69" t="s">
+        <v>558</v>
       </c>
       <c r="I69" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4522,14 +4501,14 @@
       <c r="F70" t="s">
         <v>113</v>
       </c>
-      <c r="H70" s="45" t="s">
-        <v>552</v>
+      <c r="H70" t="s">
+        <v>559</v>
       </c>
       <c r="I70" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4551,14 +4530,14 @@
       <c r="G71" s="42" t="s">
         <v>233</v>
       </c>
-      <c r="H71" s="45" t="s">
-        <v>553</v>
+      <c r="H71" t="s">
+        <v>586</v>
       </c>
       <c r="I71" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4572,7 +4551,7 @@
         <v>216</v>
       </c>
       <c r="E72" t="s">
-        <v>589</v>
+        <v>492</v>
       </c>
       <c r="F72" s="42" t="s">
         <v>232</v>
@@ -4580,14 +4559,14 @@
       <c r="G72" t="s">
         <v>234</v>
       </c>
-      <c r="H72" s="45" t="s">
-        <v>553</v>
+      <c r="H72" t="s">
+        <v>587</v>
       </c>
       <c r="I72" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4609,14 +4588,14 @@
       <c r="G73" t="s">
         <v>235</v>
       </c>
-      <c r="H73" s="45" t="s">
-        <v>554</v>
+      <c r="H73" t="s">
+        <v>560</v>
       </c>
       <c r="I73" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4630,7 +4609,7 @@
         <v>217</v>
       </c>
       <c r="E74" t="s">
-        <v>590</v>
+        <v>493</v>
       </c>
       <c r="F74" s="42" t="s">
         <v>232</v>
@@ -4638,14 +4617,14 @@
       <c r="G74" s="42" t="s">
         <v>233</v>
       </c>
-      <c r="H74" s="45" t="s">
-        <v>555</v>
+      <c r="H74" t="s">
+        <v>561</v>
       </c>
       <c r="I74" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4667,14 +4646,14 @@
       <c r="G75" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="H75" s="45" t="s">
-        <v>556</v>
+      <c r="H75" t="s">
+        <v>562</v>
       </c>
       <c r="I75" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4693,14 +4672,14 @@
       <c r="F76" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="H76" s="45" t="s">
-        <v>557</v>
+      <c r="H76" t="s">
+        <v>563</v>
       </c>
       <c r="I76" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4719,14 +4698,14 @@
       <c r="F77" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="H77" s="47" t="s">
-        <v>558</v>
+      <c r="H77" t="s">
+        <v>564</v>
       </c>
       <c r="I77" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4745,14 +4724,14 @@
       <c r="F78" t="s">
         <v>114</v>
       </c>
-      <c r="H78" s="45" t="s">
-        <v>559</v>
+      <c r="H78" t="s">
+        <v>565</v>
       </c>
       <c r="I78" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -4766,7 +4745,7 @@
         <v>170</v>
       </c>
       <c r="E79" t="s">
-        <v>588</v>
+        <v>491</v>
       </c>
       <c r="F79" t="s">
         <v>106</v>
@@ -4774,14 +4753,14 @@
       <c r="G79" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H79" s="45" t="s">
-        <v>560</v>
+      <c r="H79" t="s">
+        <v>566</v>
       </c>
       <c r="I79" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -4800,14 +4779,14 @@
       <c r="F80" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="H80" s="45" t="s">
-        <v>561</v>
+      <c r="H80" t="s">
+        <v>567</v>
       </c>
       <c r="I80" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4823,14 +4802,14 @@
       <c r="E81" t="s">
         <v>220</v>
       </c>
-      <c r="H81" s="45" t="s">
-        <v>562</v>
+      <c r="H81" t="s">
+        <v>568</v>
       </c>
       <c r="I81" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -4846,14 +4825,14 @@
       <c r="E82" t="s">
         <v>157</v>
       </c>
-      <c r="H82" s="45" t="s">
-        <v>563</v>
+      <c r="H82" t="s">
+        <v>569</v>
       </c>
       <c r="I82" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -4869,14 +4848,14 @@
       <c r="E83" t="s">
         <v>158</v>
       </c>
-      <c r="H83" s="45" t="s">
-        <v>564</v>
+      <c r="H83" t="s">
+        <v>570</v>
       </c>
       <c r="I83" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -4892,14 +4871,14 @@
       <c r="E84" t="s">
         <v>157</v>
       </c>
-      <c r="H84" s="45" t="s">
-        <v>565</v>
+      <c r="H84" t="s">
+        <v>571</v>
       </c>
       <c r="I84" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -4921,14 +4900,14 @@
       <c r="G85" t="s">
         <v>205</v>
       </c>
-      <c r="H85" s="45" t="s">
-        <v>566</v>
+      <c r="H85" t="s">
+        <v>588</v>
       </c>
       <c r="I85" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -4944,14 +4923,14 @@
       <c r="E86" t="s">
         <v>159</v>
       </c>
-      <c r="H86" s="45" t="s">
-        <v>567</v>
+      <c r="H86" t="s">
+        <v>572</v>
       </c>
       <c r="I86" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -4967,14 +4946,14 @@
       <c r="E87" t="s">
         <v>161</v>
       </c>
-      <c r="H87" s="45" t="s">
-        <v>568</v>
+      <c r="H87" t="s">
+        <v>573</v>
       </c>
       <c r="I87" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -4990,14 +4969,14 @@
       <c r="E88" t="s">
         <v>160</v>
       </c>
-      <c r="H88" s="45" t="s">
-        <v>569</v>
+      <c r="H88" t="s">
+        <v>574</v>
       </c>
       <c r="I88" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -5013,14 +4992,14 @@
       <c r="E89" t="s">
         <v>161</v>
       </c>
-      <c r="H89" s="45" t="s">
-        <v>570</v>
+      <c r="H89" t="s">
+        <v>575</v>
       </c>
       <c r="I89" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -5036,14 +5015,14 @@
       <c r="E90" t="s">
         <v>162</v>
       </c>
-      <c r="H90" s="45" t="s">
-        <v>571</v>
+      <c r="H90" t="s">
+        <v>576</v>
       </c>
       <c r="I90" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -5059,14 +5038,14 @@
       <c r="E91" t="s">
         <v>229</v>
       </c>
-      <c r="H91" s="45" t="s">
-        <v>572</v>
+      <c r="H91" t="s">
+        <v>577</v>
       </c>
       <c r="I91" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -5082,14 +5061,14 @@
       <c r="E92" t="s">
         <v>163</v>
       </c>
-      <c r="H92" s="45" t="s">
-        <v>573</v>
+      <c r="H92" t="s">
+        <v>578</v>
       </c>
       <c r="I92" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -5105,14 +5084,14 @@
       <c r="E93" t="s">
         <v>164</v>
       </c>
-      <c r="H93" s="45" t="s">
-        <v>574</v>
+      <c r="H93" t="s">
+        <v>579</v>
       </c>
       <c r="I93" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -5131,14 +5110,14 @@
       <c r="G94" t="s">
         <v>224</v>
       </c>
-      <c r="H94" s="45" t="s">
-        <v>575</v>
+      <c r="H94" t="s">
+        <v>580</v>
       </c>
       <c r="I94" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -5154,14 +5133,14 @@
       <c r="E95" t="s">
         <v>226</v>
       </c>
-      <c r="H95" s="45" t="s">
-        <v>576</v>
+      <c r="H95" t="s">
+        <v>591</v>
       </c>
       <c r="I95" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -5177,14 +5156,14 @@
       <c r="E96" t="s">
         <v>225</v>
       </c>
-      <c r="H96" s="45" t="s">
-        <v>577</v>
+      <c r="H96" t="s">
+        <v>590</v>
       </c>
       <c r="I96" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -5200,14 +5179,14 @@
       <c r="E97" t="s">
         <v>165</v>
       </c>
-      <c r="H97" s="45" t="s">
-        <v>578</v>
+      <c r="H97" t="s">
+        <v>581</v>
       </c>
       <c r="I97" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -5224,14 +5203,14 @@
         <v>236</v>
       </c>
       <c r="F98" s="43"/>
-      <c r="H98" s="45" t="s">
-        <v>579</v>
+      <c r="H98" t="s">
+        <v>582</v>
       </c>
       <c r="I98" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -5247,8 +5226,8 @@
       <c r="E99" t="s">
         <v>486</v>
       </c>
-      <c r="H99" s="48" t="s">
-        <v>580</v>
+      <c r="H99" t="s">
+        <v>589</v>
       </c>
       <c r="I99" t="s">
         <v>483</v>

</xml_diff>

<commit_message>
add a link to field values
</commit_message>
<xml_diff>
--- a/dbs/database.eamena/data/reference_data/rm/hp/mds/mds-template.xlsx
+++ b/dbs/database.eamena/data/reference_data/rm/hp/mds/mds-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rprojects\eamena-arches-dev\dbs\database.eamena\data\reference_data\rm\hp\mds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34908C02-9F92-415E-9093-6D03A8115CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A1C11E-4389-4666-A485-9B7B8A6DAD3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{1E0C3C69-C562-4061-B01F-1E26B463065A}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{1E0C3C69-C562-4061-B01F-1E26B463065A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1661,9 +1661,6 @@
     <t>Structured data. Defines certainty levels in in identifying archaeological values of heritage places. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/90' target='_blank'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
   </si>
   <si>
-    <t>Structured data. Identifies types of heritage places based on their morphology - whether they are negative/cut/dug features, constructed above ground, surface marks, or undetermined. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/91' target='_blank'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
-  </si>
-  <si>
     <t>Structured data. Classifies cultural periods of cultural heritage places from Palaeolithic to Contemporary Islamic. &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/92' target='_blank'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
   </si>
   <si>
@@ -1944,6 +1941,9 @@
   </si>
   <si>
     <t>Free text. The EPSG code of the coordinates. &lt;small&gt;&lt;b&gt;&lt;a href= 'https://eamena-project.github.io/eamena-arches-dev/dbs/database.eamena/data/reference_data/rm/hp/values/Environment_Assessment/Datum_Description_EPSG_code.html' target='_blank'&gt;values&lt;/a&gt;&lt;/b&gt;&lt;/small&gt; &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/155' target='_blank'&gt;issue&lt;/a&gt;&lt;small&gt;.</t>
+  </si>
+  <si>
+    <t>Structured data. Identifies types of heritage places based on their morphology - whether they are negative/cut/dug features, constructed above ground, surface marks, or undetermined. &lt;small&gt;&lt;b&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/blob/main/dbs/database.eamena/data/reference_data/rm/hp/values/Archaeological_Assessment/Morphology.tsv ' target='_blank'&gt;values&lt;/a&gt;&lt;/b&gt;&lt;/small&gt; &lt;small&gt;&lt;a href='https://github.com/eamena-project/eamena-arches-dev/issues/91' target='_blank'&gt;issue&lt;/a&gt;&lt;/small&gt;.</t>
   </si>
 </sst>
 </file>
@@ -2735,10 +2735,10 @@
   <dimension ref="A1:I99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="H68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="H26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H101" sqref="H101"/>
+      <selection pane="bottomRight" activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2771,7 +2771,7 @@
         <v>94</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>168</v>
@@ -2803,7 +2803,7 @@
         <v>105</v>
       </c>
       <c r="H2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I2" t="s">
         <v>243</v>
@@ -2829,7 +2829,7 @@
         <v>105</v>
       </c>
       <c r="H3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I3" t="s">
         <v>243</v>
@@ -2855,7 +2855,7 @@
         <v>112</v>
       </c>
       <c r="H4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="I4" t="s">
         <v>243</v>
@@ -2881,7 +2881,7 @@
         <v>105</v>
       </c>
       <c r="H5" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="I5" t="s">
         <v>243</v>
@@ -2956,7 +2956,7 @@
         <v>175</v>
       </c>
       <c r="H8" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I8" t="s">
         <v>261</v>
@@ -2979,7 +2979,7 @@
         <v>101</v>
       </c>
       <c r="H9" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="I9" t="s">
         <v>261</v>
@@ -3005,7 +3005,7 @@
         <v>107</v>
       </c>
       <c r="H10" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="I10" t="s">
         <v>266</v>
@@ -3031,7 +3031,7 @@
         <v>108</v>
       </c>
       <c r="H11" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I11" t="s">
         <v>266</v>
@@ -3057,7 +3057,7 @@
         <v>109</v>
       </c>
       <c r="H12" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I12" t="s">
         <v>266</v>
@@ -3083,7 +3083,7 @@
         <v>109</v>
       </c>
       <c r="H13" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="I13" t="s">
         <v>266</v>
@@ -3109,7 +3109,7 @@
         <v>109</v>
       </c>
       <c r="H14" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="I14" t="s">
         <v>266</v>
@@ -3135,7 +3135,7 @@
         <v>487</v>
       </c>
       <c r="H15" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="I15" t="s">
         <v>278</v>
@@ -3161,7 +3161,7 @@
         <v>110</v>
       </c>
       <c r="H16" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="I16" t="s">
         <v>278</v>
@@ -3187,7 +3187,7 @@
         <v>109</v>
       </c>
       <c r="H17" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I17" t="s">
         <v>266</v>
@@ -3213,7 +3213,7 @@
         <v>109</v>
       </c>
       <c r="H18" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I18" t="s">
         <v>266</v>
@@ -3239,7 +3239,7 @@
         <v>109</v>
       </c>
       <c r="H19" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="I19" t="s">
         <v>266</v>
@@ -3265,7 +3265,7 @@
         <v>105</v>
       </c>
       <c r="H20" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="I20" t="s">
         <v>291</v>
@@ -3314,7 +3314,7 @@
         <v>112</v>
       </c>
       <c r="H22" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I22" t="s">
         <v>291</v>
@@ -3340,7 +3340,7 @@
         <v>109</v>
       </c>
       <c r="H23" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="I23" t="s">
         <v>294</v>
@@ -3366,7 +3366,7 @@
         <v>108</v>
       </c>
       <c r="H24" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I24" t="s">
         <v>302</v>
@@ -3392,7 +3392,7 @@
         <v>105</v>
       </c>
       <c r="H25" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I25" t="s">
         <v>306</v>
@@ -3418,7 +3418,7 @@
         <v>112</v>
       </c>
       <c r="H26" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="I26" t="s">
         <v>306</v>
@@ -3444,7 +3444,7 @@
         <v>109</v>
       </c>
       <c r="H27" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I27" t="s">
         <v>302</v>
@@ -3470,7 +3470,7 @@
         <v>109</v>
       </c>
       <c r="H28" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="I28" t="s">
         <v>302</v>
@@ -3493,7 +3493,7 @@
         <v>126</v>
       </c>
       <c r="H29" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I29" t="s">
         <v>302</v>
@@ -3516,7 +3516,7 @@
         <v>127</v>
       </c>
       <c r="H30" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="I30" t="s">
         <v>302</v>
@@ -3539,7 +3539,7 @@
         <v>181</v>
       </c>
       <c r="H31" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="I31" t="s">
         <v>302</v>
@@ -3562,7 +3562,7 @@
         <v>182</v>
       </c>
       <c r="H32" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I32" t="s">
         <v>302</v>
@@ -3614,7 +3614,7 @@
         <v>105</v>
       </c>
       <c r="H34" t="s">
-        <v>497</v>
+        <v>591</v>
       </c>
       <c r="I34" t="s">
         <v>325</v>
@@ -3640,7 +3640,7 @@
         <v>488</v>
       </c>
       <c r="H35" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="I35" t="s">
         <v>325</v>
@@ -3666,7 +3666,7 @@
         <v>105</v>
       </c>
       <c r="H36" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I36" t="s">
         <v>325</v>
@@ -3692,7 +3692,7 @@
         <v>109</v>
       </c>
       <c r="H37" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="I37" t="s">
         <v>337</v>
@@ -3718,7 +3718,7 @@
         <v>109</v>
       </c>
       <c r="H38" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I38" t="s">
         <v>337</v>
@@ -3741,7 +3741,7 @@
         <v>131</v>
       </c>
       <c r="H39" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="I39" t="s">
         <v>337</v>
@@ -3764,7 +3764,7 @@
         <v>192</v>
       </c>
       <c r="H40" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I40" t="s">
         <v>337</v>
@@ -3787,7 +3787,7 @@
         <v>193</v>
       </c>
       <c r="H41" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I41" t="s">
         <v>337</v>
@@ -3810,7 +3810,7 @@
         <v>132</v>
       </c>
       <c r="H42" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="I42" t="s">
         <v>337</v>
@@ -3833,7 +3833,7 @@
         <v>133</v>
       </c>
       <c r="H43" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I43" t="s">
         <v>337</v>
@@ -3856,7 +3856,7 @@
         <v>134</v>
       </c>
       <c r="H44" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I44" t="s">
         <v>337</v>
@@ -3879,7 +3879,7 @@
         <v>135</v>
       </c>
       <c r="H45" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I45" t="s">
         <v>337</v>
@@ -3902,7 +3902,7 @@
         <v>136</v>
       </c>
       <c r="H46" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="I46" t="s">
         <v>337</v>
@@ -3925,7 +3925,7 @@
         <v>196</v>
       </c>
       <c r="H47" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="I47" t="s">
         <v>337</v>
@@ -3951,7 +3951,7 @@
         <v>111</v>
       </c>
       <c r="H48" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I48" t="s">
         <v>337</v>
@@ -3977,7 +3977,7 @@
         <v>108</v>
       </c>
       <c r="H49" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="I49" t="s">
         <v>337</v>
@@ -4003,7 +4003,7 @@
         <v>109</v>
       </c>
       <c r="H50" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="I50" t="s">
         <v>337</v>
@@ -4029,7 +4029,7 @@
         <v>109</v>
       </c>
       <c r="H51" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="I51" t="s">
         <v>337</v>
@@ -4055,7 +4055,7 @@
         <v>109</v>
       </c>
       <c r="H52" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I52" t="s">
         <v>337</v>
@@ -4081,7 +4081,7 @@
         <v>489</v>
       </c>
       <c r="H53" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I53" t="s">
         <v>325</v>
@@ -4107,7 +4107,7 @@
         <v>105</v>
       </c>
       <c r="H54" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I54" t="s">
         <v>325</v>
@@ -4133,7 +4133,7 @@
         <v>105</v>
       </c>
       <c r="H55" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="I55" t="s">
         <v>325</v>
@@ -4159,7 +4159,7 @@
         <v>204</v>
       </c>
       <c r="H56" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="I56" t="s">
         <v>337</v>
@@ -4185,7 +4185,7 @@
         <v>204</v>
       </c>
       <c r="H57" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="I57" t="s">
         <v>337</v>
@@ -4208,7 +4208,7 @@
         <v>143</v>
       </c>
       <c r="H58" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I58" t="s">
         <v>337</v>
@@ -4231,7 +4231,7 @@
         <v>144</v>
       </c>
       <c r="H59" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="I59" t="s">
         <v>337</v>
@@ -4254,7 +4254,7 @@
         <v>145</v>
       </c>
       <c r="H60" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="I60" t="s">
         <v>337</v>
@@ -4277,7 +4277,7 @@
         <v>146</v>
       </c>
       <c r="H61" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="I61" t="s">
         <v>337</v>
@@ -4300,7 +4300,7 @@
         <v>147</v>
       </c>
       <c r="H62" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="I62" t="s">
         <v>337</v>
@@ -4323,7 +4323,7 @@
         <v>148</v>
       </c>
       <c r="H63" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="I63" t="s">
         <v>337</v>
@@ -4346,7 +4346,7 @@
         <v>205</v>
       </c>
       <c r="H64" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I64" t="s">
         <v>337</v>
@@ -4372,7 +4372,7 @@
         <v>109</v>
       </c>
       <c r="H65" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="I65" t="s">
         <v>337</v>
@@ -4398,7 +4398,7 @@
         <v>112</v>
       </c>
       <c r="H66" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="I66" t="s">
         <v>400</v>
@@ -4424,7 +4424,7 @@
         <v>109</v>
       </c>
       <c r="H67" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="I67" t="s">
         <v>403</v>
@@ -4450,7 +4450,7 @@
         <v>112</v>
       </c>
       <c r="H68" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="I68" t="s">
         <v>400</v>
@@ -4476,7 +4476,7 @@
         <v>112</v>
       </c>
       <c r="H69" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="I69" t="s">
         <v>400</v>
@@ -4502,7 +4502,7 @@
         <v>112</v>
       </c>
       <c r="H70" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="I70" t="s">
         <v>400</v>
@@ -4531,7 +4531,7 @@
         <v>232</v>
       </c>
       <c r="H71" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I71" t="s">
         <v>400</v>
@@ -4560,7 +4560,7 @@
         <v>233</v>
       </c>
       <c r="H72" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="I72" t="s">
         <v>400</v>
@@ -4589,7 +4589,7 @@
         <v>234</v>
       </c>
       <c r="H73" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="I73" t="s">
         <v>400</v>
@@ -4618,7 +4618,7 @@
         <v>232</v>
       </c>
       <c r="H74" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="I74" t="s">
         <v>400</v>
@@ -4647,7 +4647,7 @@
         <v>73</v>
       </c>
       <c r="H75" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I75" t="s">
         <v>403</v>
@@ -4673,7 +4673,7 @@
         <v>112</v>
       </c>
       <c r="H76" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="I76" t="s">
         <v>400</v>
@@ -4699,7 +4699,7 @@
         <v>105</v>
       </c>
       <c r="H77" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="I77" t="s">
         <v>400</v>
@@ -4725,7 +4725,7 @@
         <v>113</v>
       </c>
       <c r="H78" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="I78" t="s">
         <v>400</v>
@@ -4754,7 +4754,7 @@
         <v>77</v>
       </c>
       <c r="H79" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I79" t="s">
         <v>400</v>
@@ -4780,7 +4780,7 @@
         <v>112</v>
       </c>
       <c r="H80" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I80" t="s">
         <v>400</v>
@@ -4803,7 +4803,7 @@
         <v>219</v>
       </c>
       <c r="H81" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="I81" t="s">
         <v>403</v>
@@ -4826,7 +4826,7 @@
         <v>156</v>
       </c>
       <c r="H82" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I82" t="s">
         <v>403</v>
@@ -4849,7 +4849,7 @@
         <v>157</v>
       </c>
       <c r="H83" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="I83" t="s">
         <v>403</v>
@@ -4872,7 +4872,7 @@
         <v>156</v>
       </c>
       <c r="H84" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="I84" t="s">
         <v>403</v>
@@ -4901,7 +4901,7 @@
         <v>204</v>
       </c>
       <c r="H85" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="I85" t="s">
         <v>403</v>
@@ -4924,7 +4924,7 @@
         <v>158</v>
       </c>
       <c r="H86" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I86" t="s">
         <v>455</v>
@@ -4947,7 +4947,7 @@
         <v>160</v>
       </c>
       <c r="H87" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I87" t="s">
         <v>455</v>
@@ -4970,7 +4970,7 @@
         <v>159</v>
       </c>
       <c r="H88" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="I88" t="s">
         <v>455</v>
@@ -4993,7 +4993,7 @@
         <v>160</v>
       </c>
       <c r="H89" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="I89" t="s">
         <v>455</v>
@@ -5016,7 +5016,7 @@
         <v>161</v>
       </c>
       <c r="H90" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="I90" t="s">
         <v>455</v>
@@ -5039,7 +5039,7 @@
         <v>228</v>
       </c>
       <c r="H91" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="I91" t="s">
         <v>455</v>
@@ -5062,7 +5062,7 @@
         <v>162</v>
       </c>
       <c r="H92" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="I92" t="s">
         <v>455</v>
@@ -5085,7 +5085,7 @@
         <v>163</v>
       </c>
       <c r="H93" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I93" t="s">
         <v>455</v>
@@ -5111,7 +5111,7 @@
         <v>223</v>
       </c>
       <c r="H94" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I94" t="s">
         <v>455</v>
@@ -5134,7 +5134,7 @@
         <v>225</v>
       </c>
       <c r="H95" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="I95" t="s">
         <v>455</v>
@@ -5157,7 +5157,7 @@
         <v>224</v>
       </c>
       <c r="H96" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="I96" t="s">
         <v>455</v>
@@ -5180,7 +5180,7 @@
         <v>164</v>
       </c>
       <c r="H97" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="I97" t="s">
         <v>455</v>
@@ -5204,7 +5204,7 @@
       </c>
       <c r="F98" s="43"/>
       <c r="H98" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="I98" t="s">
         <v>455</v>
@@ -5227,7 +5227,7 @@
         <v>485</v>
       </c>
       <c r="H99" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="I99" t="s">
         <v>482</v>

</xml_diff>